<commit_message>
Finished Calculating Histograms of particles Before and After LTD keeping only the ones close to synpases
</commit_message>
<xml_diff>
--- a/cluster/distance change/dist-homer-ampar-after-ctr-1.xlsx
+++ b/cluster/distance change/dist-homer-ampar-after-ctr-1.xlsx
@@ -398,7 +398,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:J151"/>
+  <dimension ref="A1:J150"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -2323,2913 +2323,2881 @@
     </row>
     <row r="61" spans="1:10">
       <c r="A61" s="1">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="B61">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="C61">
-        <v>8336.294613085764</v>
+        <v>38005.69212032654</v>
       </c>
       <c r="D61">
-        <v>34067.36621864088</v>
+        <v>36669.0848733647</v>
       </c>
       <c r="E61">
-        <v>48.36653242951991</v>
+        <v>152.20850018664</v>
       </c>
       <c r="F61">
-        <v>1225</v>
+        <v>677</v>
       </c>
       <c r="G61">
-        <v>8435.308014382354</v>
+        <v>37272.86753739131</v>
       </c>
       <c r="H61">
-        <v>34526.04412235294</v>
+        <v>36110.06571956522</v>
       </c>
       <c r="I61">
-        <v>23.00235260181794</v>
+        <v>223.8359628803913</v>
       </c>
       <c r="J61">
-        <v>469.9280951468419</v>
+        <v>924.4808148798118</v>
       </c>
     </row>
     <row r="62" spans="1:10">
       <c r="A62" s="1">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="B62">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="C62">
-        <v>38005.69212032654</v>
+        <v>40383.86889383879</v>
       </c>
       <c r="D62">
-        <v>36669.0848733647</v>
+        <v>52212.73317364998</v>
       </c>
       <c r="E62">
-        <v>152.20850018664</v>
+        <v>3.102920916767573</v>
       </c>
       <c r="F62">
-        <v>677</v>
+        <v>703</v>
       </c>
       <c r="G62">
-        <v>37272.86753739131</v>
+        <v>40143.57674545454</v>
       </c>
       <c r="H62">
-        <v>36110.06571956522</v>
+        <v>52468.53862454545</v>
       </c>
       <c r="I62">
-        <v>223.8359628803913</v>
+        <v>-51.56662067379091</v>
       </c>
       <c r="J62">
-        <v>924.4808148798118</v>
+        <v>355.1978379166604</v>
       </c>
     </row>
     <row r="63" spans="1:10">
       <c r="A63" s="1">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="B63">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="C63">
-        <v>40383.86889383879</v>
+        <v>62927.40365868045</v>
       </c>
       <c r="D63">
-        <v>52212.73317364998</v>
+        <v>71219.79433685591</v>
       </c>
       <c r="E63">
-        <v>3.102920916767573</v>
+        <v>204.8041485555519</v>
       </c>
       <c r="F63">
-        <v>703</v>
+        <v>1925</v>
       </c>
       <c r="G63">
-        <v>40143.57674545454</v>
+        <v>63521.919256</v>
       </c>
       <c r="H63">
-        <v>52468.53862454545</v>
+        <v>71592.31541700001</v>
       </c>
       <c r="I63">
-        <v>-51.56662067379091</v>
+        <v>215.7783974879</v>
       </c>
       <c r="J63">
-        <v>355.1978379166604</v>
+        <v>701.6702820752618</v>
       </c>
     </row>
     <row r="64" spans="1:10">
       <c r="A64" s="1">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="B64">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="C64">
-        <v>62927.40365868045</v>
+        <v>17223.84369592039</v>
       </c>
       <c r="D64">
-        <v>71219.79433685591</v>
+        <v>30597.06465021366</v>
       </c>
       <c r="E64">
-        <v>204.8041485555519</v>
+        <v>61.37347029910793</v>
       </c>
       <c r="F64">
-        <v>1925</v>
+        <v>46</v>
       </c>
       <c r="G64">
-        <v>63521.919256</v>
+        <v>16780.52401102678</v>
       </c>
       <c r="H64">
-        <v>71592.31541700001</v>
+        <v>30073.43229854911</v>
       </c>
       <c r="I64">
-        <v>215.7783974879</v>
+        <v>154.8499557368185</v>
       </c>
       <c r="J64">
-        <v>701.6702820752618</v>
+        <v>692.4312500557022</v>
       </c>
     </row>
     <row r="65" spans="1:10">
       <c r="A65" s="1">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="B65">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="C65">
-        <v>17223.84369592039</v>
+        <v>27872.51420577471</v>
       </c>
       <c r="D65">
-        <v>30597.06465021366</v>
+        <v>29205.64386533108</v>
       </c>
       <c r="E65">
-        <v>61.37347029910793</v>
+        <v>20.84921311667322</v>
       </c>
       <c r="F65">
-        <v>46</v>
+        <v>1970</v>
       </c>
       <c r="G65">
-        <v>16780.52401102678</v>
+        <v>27977.92028128205</v>
       </c>
       <c r="H65">
-        <v>30073.43229854911</v>
+        <v>29431.7885174359</v>
       </c>
       <c r="I65">
-        <v>154.8499557368185</v>
+        <v>78.78837762803795</v>
       </c>
       <c r="J65">
-        <v>692.4312500557022</v>
+        <v>256.1421308838987</v>
       </c>
     </row>
     <row r="66" spans="1:10">
       <c r="A66" s="1">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="B66">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="C66">
-        <v>27872.51420577471</v>
+        <v>13898.48320447491</v>
       </c>
       <c r="D66">
-        <v>29205.64386533108</v>
+        <v>50311.25823938216</v>
       </c>
       <c r="E66">
-        <v>20.84921311667322</v>
+        <v>253.9797628689115</v>
       </c>
       <c r="F66">
-        <v>1970</v>
+        <v>1503</v>
       </c>
       <c r="G66">
-        <v>27977.92028128205</v>
+        <v>14015.92716727273</v>
       </c>
       <c r="H66">
-        <v>29431.7885174359</v>
+        <v>50220.98823090909</v>
       </c>
       <c r="I66">
-        <v>78.78837762803795</v>
+        <v>-12.72536071484045</v>
       </c>
       <c r="J66">
-        <v>256.1421308838987</v>
+        <v>305.0793040722502</v>
       </c>
     </row>
     <row r="67" spans="1:10">
       <c r="A67" s="1">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="B67">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="C67">
-        <v>13898.48320447491</v>
+        <v>35863.76019858087</v>
       </c>
       <c r="D67">
-        <v>50311.25823938216</v>
+        <v>73762.4191747032</v>
       </c>
       <c r="E67">
-        <v>253.9797628689115</v>
+        <v>239.2071277411486</v>
       </c>
       <c r="F67">
-        <v>1503</v>
+        <v>39</v>
       </c>
       <c r="G67">
-        <v>14015.92716727273</v>
+        <v>35781.57730314</v>
       </c>
       <c r="H67">
-        <v>50220.98823090909</v>
+        <v>73854.68779086</v>
       </c>
       <c r="I67">
-        <v>-12.72536071484045</v>
+        <v>157.038698162016</v>
       </c>
       <c r="J67">
-        <v>305.0793040722502</v>
+        <v>148.3886001350387</v>
       </c>
     </row>
     <row r="68" spans="1:10">
       <c r="A68" s="1">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="B68">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="C68">
-        <v>35863.76019858087</v>
+        <v>75954.82220196964</v>
       </c>
       <c r="D68">
-        <v>73762.4191747032</v>
+        <v>70970.32734519962</v>
       </c>
       <c r="E68">
-        <v>239.2071277411486</v>
+        <v>190.5510142535862</v>
       </c>
       <c r="F68">
-        <v>39</v>
+        <v>106</v>
       </c>
       <c r="G68">
-        <v>35781.57730314</v>
+        <v>75701.86304847999</v>
       </c>
       <c r="H68">
-        <v>73854.68779086</v>
+        <v>70718.51912174</v>
       </c>
       <c r="I68">
-        <v>157.038698162016</v>
+        <v>-71.55296774316162</v>
       </c>
       <c r="J68">
-        <v>148.3886001350387</v>
+        <v>442.8252613781659</v>
       </c>
     </row>
     <row r="69" spans="1:10">
       <c r="A69" s="1">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="B69">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="C69">
-        <v>75954.82220196964</v>
+        <v>20548.66308274763</v>
       </c>
       <c r="D69">
-        <v>70970.32734519962</v>
+        <v>61073.43121649307</v>
       </c>
       <c r="E69">
-        <v>190.5510142535862</v>
+        <v>121.588535772778</v>
       </c>
       <c r="F69">
-        <v>106</v>
+        <v>1698</v>
       </c>
       <c r="G69">
-        <v>75701.86304847999</v>
+        <v>20180.85517244681</v>
       </c>
       <c r="H69">
-        <v>70718.51912174</v>
+        <v>61459.94949819149</v>
       </c>
       <c r="I69">
-        <v>-71.55296774316162</v>
+        <v>272.8018147405745</v>
       </c>
       <c r="J69">
-        <v>442.8252613781659</v>
+        <v>554.5669451952058</v>
       </c>
     </row>
     <row r="70" spans="1:10">
       <c r="A70" s="1">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="B70">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="C70">
-        <v>20548.66308274763</v>
+        <v>29693.0687864371</v>
       </c>
       <c r="D70">
-        <v>61073.43121649307</v>
+        <v>13381.01515018709</v>
       </c>
       <c r="E70">
-        <v>121.588535772778</v>
+        <v>154.7897732811778</v>
       </c>
       <c r="F70">
-        <v>1698</v>
+        <v>1455</v>
       </c>
       <c r="G70">
-        <v>20180.85517244681</v>
+        <v>29347.57089941177</v>
       </c>
       <c r="H70">
-        <v>61459.94949819149</v>
+        <v>13169.15930941177</v>
       </c>
       <c r="I70">
-        <v>272.8018147405745</v>
+        <v>373.1822169675883</v>
       </c>
       <c r="J70">
-        <v>554.5669451952058</v>
+        <v>460.3769614879882</v>
       </c>
     </row>
     <row r="71" spans="1:10">
       <c r="A71" s="1">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="B71">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="C71">
-        <v>29693.0687864371</v>
+        <v>6904.269242955167</v>
       </c>
       <c r="D71">
-        <v>13381.01515018709</v>
+        <v>7822.531916978472</v>
       </c>
       <c r="E71">
-        <v>154.7897732811778</v>
+        <v>152.129334467964</v>
       </c>
       <c r="F71">
-        <v>1455</v>
+        <v>1931</v>
       </c>
       <c r="G71">
-        <v>29347.57089941177</v>
+        <v>6873.735578466667</v>
       </c>
       <c r="H71">
-        <v>13169.15930941177</v>
+        <v>7844.427783733333</v>
       </c>
       <c r="I71">
-        <v>373.1822169675883</v>
+        <v>-67.60027343651333</v>
       </c>
       <c r="J71">
-        <v>460.3769614879882</v>
+        <v>222.9188960987791</v>
       </c>
     </row>
     <row r="72" spans="1:10">
       <c r="A72" s="1">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="B72">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="C72">
-        <v>6904.269242955167</v>
+        <v>27158.38708120425</v>
       </c>
       <c r="D72">
-        <v>7822.531916978472</v>
+        <v>13530.17463463211</v>
       </c>
       <c r="E72">
-        <v>152.129334467964</v>
+        <v>346.1734623208576</v>
       </c>
       <c r="F72">
-        <v>1931</v>
+        <v>1517</v>
       </c>
       <c r="G72">
-        <v>6873.735578466667</v>
+        <v>26666.90476791667</v>
       </c>
       <c r="H72">
-        <v>7844.427783733333</v>
+        <v>13736.41778569444</v>
       </c>
       <c r="I72">
-        <v>-67.60027343651333</v>
+        <v>248.8221621626875</v>
       </c>
       <c r="J72">
-        <v>222.9188960987791</v>
+        <v>541.8195061799813</v>
       </c>
     </row>
     <row r="73" spans="1:10">
       <c r="A73" s="1">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="B73">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="C73">
-        <v>27158.38708120425</v>
+        <v>5200.958820813859</v>
       </c>
       <c r="D73">
-        <v>13530.17463463211</v>
+        <v>23260.76415616143</v>
       </c>
       <c r="E73">
-        <v>346.1734623208576</v>
+        <v>135.6382782640792</v>
       </c>
       <c r="F73">
-        <v>1517</v>
+        <v>449</v>
       </c>
       <c r="G73">
-        <v>26666.90476791667</v>
+        <v>5815.642716</v>
       </c>
       <c r="H73">
-        <v>13736.41778569444</v>
+        <v>22673.4639952381</v>
       </c>
       <c r="I73">
-        <v>248.8221621626875</v>
+        <v>55.55577877922904</v>
       </c>
       <c r="J73">
-        <v>541.8195061799813</v>
+        <v>853.9150875500001</v>
       </c>
     </row>
     <row r="74" spans="1:10">
       <c r="A74" s="1">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="B74">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="C74">
-        <v>5200.958820813859</v>
+        <v>36706.7610769003</v>
       </c>
       <c r="D74">
-        <v>23260.76415616143</v>
+        <v>48673.97809285378</v>
       </c>
       <c r="E74">
-        <v>135.6382782640792</v>
+        <v>137.7803368086704</v>
       </c>
       <c r="F74">
-        <v>449</v>
+        <v>1525</v>
       </c>
       <c r="G74">
-        <v>5815.642716</v>
+        <v>37030.50612561798</v>
       </c>
       <c r="H74">
-        <v>22673.4639952381</v>
+        <v>49340.59489269663</v>
       </c>
       <c r="I74">
-        <v>55.55577877922904</v>
+        <v>20.68841597542741</v>
       </c>
       <c r="J74">
-        <v>853.9150875500001</v>
+        <v>750.2661743183888</v>
       </c>
     </row>
     <row r="75" spans="1:10">
       <c r="A75" s="1">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="B75">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="C75">
-        <v>36706.7610769003</v>
+        <v>9537.558756011316</v>
       </c>
       <c r="D75">
-        <v>48673.97809285378</v>
+        <v>42088.62424470185</v>
       </c>
       <c r="E75">
-        <v>137.7803368086704</v>
+        <v>107.1800827866282</v>
       </c>
       <c r="F75">
-        <v>1525</v>
+        <v>21</v>
       </c>
       <c r="G75">
-        <v>37030.50612561798</v>
+        <v>9378.578876896552</v>
       </c>
       <c r="H75">
-        <v>49340.59489269663</v>
+        <v>41499.1137675862</v>
       </c>
       <c r="I75">
-        <v>20.68841597542741</v>
+        <v>68.95191922907587</v>
       </c>
       <c r="J75">
-        <v>750.2661743183888</v>
+        <v>611.7667832446008</v>
       </c>
     </row>
     <row r="76" spans="1:10">
       <c r="A76" s="1">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="B76">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="C76">
-        <v>9537.558756011316</v>
+        <v>73452.41816162644</v>
       </c>
       <c r="D76">
-        <v>42088.62424470185</v>
+        <v>80755.35686736486</v>
       </c>
       <c r="E76">
-        <v>107.1800827866282</v>
+        <v>222.3212321060244</v>
       </c>
       <c r="F76">
-        <v>21</v>
+        <v>1514</v>
       </c>
       <c r="G76">
-        <v>9378.578876896552</v>
+        <v>73250.62670080808</v>
       </c>
       <c r="H76">
-        <v>41499.1137675862</v>
+        <v>80666.63208565656</v>
       </c>
       <c r="I76">
-        <v>68.95191922907587</v>
+        <v>68.24438918990394</v>
       </c>
       <c r="J76">
-        <v>611.7667832446008</v>
+        <v>268.9452622215031</v>
       </c>
     </row>
     <row r="77" spans="1:10">
       <c r="A77" s="1">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="B77">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="C77">
-        <v>73452.41816162644</v>
+        <v>54180.8983390537</v>
       </c>
       <c r="D77">
-        <v>80755.35686736486</v>
+        <v>56359.93399064996</v>
       </c>
       <c r="E77">
-        <v>222.3212321060244</v>
+        <v>-120.7640822514014</v>
       </c>
       <c r="F77">
-        <v>1514</v>
+        <v>248</v>
       </c>
       <c r="G77">
-        <v>73250.62670080808</v>
+        <v>54093.9342325</v>
       </c>
       <c r="H77">
-        <v>80666.63208565656</v>
+        <v>56078.25520694737</v>
       </c>
       <c r="I77">
-        <v>68.24438918990394</v>
+        <v>-173.5535425592816</v>
       </c>
       <c r="J77">
-        <v>268.9452622215031</v>
+        <v>299.4869281562226</v>
       </c>
     </row>
     <row r="78" spans="1:10">
       <c r="A78" s="1">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="B78">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="C78">
-        <v>54180.8983390537</v>
+        <v>58686.27606835819</v>
       </c>
       <c r="D78">
-        <v>56359.93399064996</v>
+        <v>69043.02517327576</v>
       </c>
       <c r="E78">
-        <v>-120.7640822514014</v>
+        <v>166.4465527383444</v>
       </c>
       <c r="F78">
-        <v>248</v>
+        <v>1197</v>
       </c>
       <c r="G78">
-        <v>54093.9342325</v>
+        <v>59724.88628611111</v>
       </c>
       <c r="H78">
-        <v>56078.25520694737</v>
+        <v>69413.98349722222</v>
       </c>
       <c r="I78">
-        <v>-173.5535425592816</v>
+        <v>-98.87328433958389</v>
       </c>
       <c r="J78">
-        <v>299.4869281562226</v>
+        <v>1134.334993938298</v>
       </c>
     </row>
     <row r="79" spans="1:10">
       <c r="A79" s="1">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="B79">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="C79">
-        <v>58686.27606835819</v>
+        <v>24379.89672591783</v>
       </c>
       <c r="D79">
-        <v>69043.02517327576</v>
+        <v>77017.18982455805</v>
       </c>
       <c r="E79">
-        <v>166.4465527383444</v>
+        <v>6.224276525590257</v>
       </c>
       <c r="F79">
-        <v>1197</v>
+        <v>50</v>
       </c>
       <c r="G79">
-        <v>59724.88628611111</v>
+        <v>24598.97218094</v>
       </c>
       <c r="H79">
-        <v>69413.98349722222</v>
+        <v>77776.54920762</v>
       </c>
       <c r="I79">
-        <v>-98.87328433958389</v>
+        <v>-11.05339745291814</v>
       </c>
       <c r="J79">
-        <v>1134.334993938298</v>
+        <v>790.5183398603117</v>
       </c>
     </row>
     <row r="80" spans="1:10">
       <c r="A80" s="1">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="B80">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="C80">
-        <v>24379.89672591783</v>
+        <v>24767.76293578879</v>
       </c>
       <c r="D80">
-        <v>77017.18982455805</v>
+        <v>79045.08287543639</v>
       </c>
       <c r="E80">
-        <v>6.224276525590257</v>
+        <v>94.98405621970949</v>
       </c>
       <c r="F80">
-        <v>50</v>
+        <v>6</v>
       </c>
       <c r="G80">
-        <v>24598.97218094</v>
+        <v>24781.31422331959</v>
       </c>
       <c r="H80">
-        <v>77776.54920762</v>
+        <v>79284.28828243299</v>
       </c>
       <c r="I80">
-        <v>-11.05339745291814</v>
+        <v>48.2673826265725</v>
       </c>
       <c r="J80">
-        <v>790.5183398603117</v>
+        <v>244.1010276950043</v>
       </c>
     </row>
     <row r="81" spans="1:10">
       <c r="A81" s="1">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="B81">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="C81">
-        <v>24767.76293578879</v>
+        <v>47983.31676208541</v>
       </c>
       <c r="D81">
-        <v>79045.08287543639</v>
+        <v>19812.34814463648</v>
       </c>
       <c r="E81">
-        <v>94.98405621970949</v>
+        <v>199.8586991134647</v>
       </c>
       <c r="F81">
-        <v>6</v>
+        <v>233</v>
       </c>
       <c r="G81">
-        <v>24781.31422331959</v>
+        <v>48854.47905047619</v>
       </c>
       <c r="H81">
-        <v>79284.28828243299</v>
+        <v>20512.48889666667</v>
       </c>
       <c r="I81">
-        <v>48.2673826265725</v>
+        <v>346.8238309513334</v>
       </c>
       <c r="J81">
-        <v>244.1010276950043</v>
+        <v>1127.261972810127</v>
       </c>
     </row>
     <row r="82" spans="1:10">
       <c r="A82" s="1">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="B82">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="C82">
-        <v>47983.31676208541</v>
+        <v>64461.20501815242</v>
       </c>
       <c r="D82">
-        <v>19812.34814463648</v>
+        <v>58033.612928887</v>
       </c>
       <c r="E82">
-        <v>199.8586991134647</v>
+        <v>-62.37168115865882</v>
       </c>
       <c r="F82">
-        <v>233</v>
+        <v>41</v>
       </c>
       <c r="G82">
-        <v>48854.47905047619</v>
+        <v>64576.60307316633</v>
       </c>
       <c r="H82">
-        <v>20512.48889666667</v>
+        <v>58160.18752388778</v>
       </c>
       <c r="I82">
-        <v>346.8238309513334</v>
+        <v>-15.4751550223801</v>
       </c>
       <c r="J82">
-        <v>1127.261972810127</v>
+        <v>177.5869459286247</v>
       </c>
     </row>
     <row r="83" spans="1:10">
       <c r="A83" s="1">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="B83">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="C83">
-        <v>64461.20501815242</v>
+        <v>10030.59293906691</v>
       </c>
       <c r="D83">
-        <v>58033.612928887</v>
+        <v>10663.24095687094</v>
       </c>
       <c r="E83">
-        <v>-62.37168115865882</v>
+        <v>27.82642778355431</v>
       </c>
       <c r="F83">
-        <v>41</v>
+        <v>1799</v>
       </c>
       <c r="G83">
-        <v>64576.60307316633</v>
+        <v>10361.91943366667</v>
       </c>
       <c r="H83">
-        <v>58160.18752388778</v>
+        <v>9643.891554333333</v>
       </c>
       <c r="I83">
-        <v>-15.4751550223801</v>
+        <v>-19.729784182188</v>
       </c>
       <c r="J83">
-        <v>177.5869459286247</v>
+        <v>1072.898897275074</v>
       </c>
     </row>
     <row r="84" spans="1:10">
       <c r="A84" s="1">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="B84">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="C84">
-        <v>10030.59293906691</v>
+        <v>46717.81901953259</v>
       </c>
       <c r="D84">
-        <v>10663.24095687094</v>
+        <v>41008.20266172586</v>
       </c>
       <c r="E84">
-        <v>27.82642778355431</v>
+        <v>121.1801937658823</v>
       </c>
       <c r="F84">
-        <v>1799</v>
+        <v>1498</v>
       </c>
       <c r="G84">
-        <v>10361.91943366667</v>
+        <v>46965.44250076923</v>
       </c>
       <c r="H84">
-        <v>9643.891554333333</v>
+        <v>40982.52789769231</v>
       </c>
       <c r="I84">
-        <v>-19.729784182188</v>
+        <v>150.3982578457692</v>
       </c>
       <c r="J84">
-        <v>1072.898897275074</v>
+        <v>250.6596841067792</v>
       </c>
     </row>
     <row r="85" spans="1:10">
       <c r="A85" s="1">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="B85">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="C85">
-        <v>46717.81901953259</v>
+        <v>30227.01745610973</v>
       </c>
       <c r="D85">
-        <v>41008.20266172586</v>
+        <v>28498.18443120487</v>
       </c>
       <c r="E85">
-        <v>121.1801937658823</v>
+        <v>-37.09823030485512</v>
       </c>
       <c r="F85">
-        <v>1498</v>
+        <v>35</v>
       </c>
       <c r="G85">
-        <v>46965.44250076923</v>
+        <v>30031.19812154</v>
       </c>
       <c r="H85">
-        <v>40982.52789769231</v>
+        <v>28683.204021</v>
       </c>
       <c r="I85">
-        <v>150.3982578457692</v>
+        <v>0.08584612975053818</v>
       </c>
       <c r="J85">
-        <v>250.6596841067792</v>
+        <v>271.9560919332125</v>
       </c>
     </row>
     <row r="86" spans="1:10">
       <c r="A86" s="1">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="B86">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="C86">
-        <v>30227.01745610973</v>
+        <v>43383.5397313915</v>
       </c>
       <c r="D86">
-        <v>28498.18443120487</v>
+        <v>54373.38161498299</v>
       </c>
       <c r="E86">
-        <v>-37.09823030485512</v>
+        <v>-66.49028024435279</v>
       </c>
       <c r="F86">
-        <v>35</v>
+        <v>1737</v>
       </c>
       <c r="G86">
-        <v>30031.19812154</v>
+        <v>42936.93700153846</v>
       </c>
       <c r="H86">
-        <v>28683.204021</v>
+        <v>54695.75476307692</v>
       </c>
       <c r="I86">
-        <v>0.08584612975053818</v>
+        <v>-49.88039383096539</v>
       </c>
       <c r="J86">
-        <v>271.9560919332125</v>
+        <v>551.0483946540804</v>
       </c>
     </row>
     <row r="87" spans="1:10">
       <c r="A87" s="1">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="B87">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="C87">
-        <v>43383.5397313915</v>
+        <v>19718.235922647</v>
       </c>
       <c r="D87">
-        <v>54373.38161498299</v>
+        <v>15700.64929350349</v>
       </c>
       <c r="E87">
-        <v>-66.49028024435279</v>
+        <v>101.3286917624915</v>
       </c>
       <c r="F87">
-        <v>1737</v>
+        <v>176</v>
       </c>
       <c r="G87">
-        <v>42936.93700153846</v>
+        <v>19620.62915369198</v>
       </c>
       <c r="H87">
-        <v>54695.75476307692</v>
+        <v>15686.33540592827</v>
       </c>
       <c r="I87">
-        <v>-49.88039383096539</v>
+        <v>36.79090636719499</v>
       </c>
       <c r="J87">
-        <v>551.0483946540804</v>
+        <v>117.8859383772485</v>
       </c>
     </row>
     <row r="88" spans="1:10">
       <c r="A88" s="1">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="B88">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="C88">
-        <v>19718.235922647</v>
+        <v>52659.54483246106</v>
       </c>
       <c r="D88">
-        <v>15700.64929350349</v>
+        <v>44647.74134140143</v>
       </c>
       <c r="E88">
-        <v>101.3286917624915</v>
+        <v>138.6304117171549</v>
       </c>
       <c r="F88">
-        <v>176</v>
+        <v>1</v>
       </c>
       <c r="G88">
-        <v>19620.62915369198</v>
+        <v>52070.43990019867</v>
       </c>
       <c r="H88">
-        <v>15686.33540592827</v>
+        <v>44614.16397474614</v>
       </c>
       <c r="I88">
-        <v>36.79090636719499</v>
+        <v>151.7061848140484</v>
       </c>
       <c r="J88">
-        <v>117.8859383772485</v>
+        <v>590.2059272910241</v>
       </c>
     </row>
     <row r="89" spans="1:10">
       <c r="A89" s="1">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="B89">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="C89">
-        <v>52659.54483246106</v>
+        <v>23503.88879842273</v>
       </c>
       <c r="D89">
-        <v>44647.74134140143</v>
+        <v>36737.43944111526</v>
       </c>
       <c r="E89">
-        <v>138.6304117171549</v>
+        <v>69.16894189313152</v>
       </c>
       <c r="F89">
-        <v>1</v>
+        <v>1075</v>
       </c>
       <c r="G89">
-        <v>52070.43990019867</v>
+        <v>23443.39439124463</v>
       </c>
       <c r="H89">
-        <v>44614.16397474614</v>
+        <v>36609.13463150214</v>
       </c>
       <c r="I89">
-        <v>151.7061848140484</v>
+        <v>46.1729408491099</v>
       </c>
       <c r="J89">
-        <v>590.2059272910241</v>
+        <v>143.7028654331695</v>
       </c>
     </row>
     <row r="90" spans="1:10">
       <c r="A90" s="1">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="B90">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="C90">
-        <v>23503.88879842273</v>
+        <v>79048.42849437706</v>
       </c>
       <c r="D90">
-        <v>36737.43944111526</v>
+        <v>44320.21433078919</v>
       </c>
       <c r="E90">
-        <v>69.16894189313152</v>
+        <v>329.7085657244825</v>
       </c>
       <c r="F90">
-        <v>1075</v>
+        <v>81</v>
       </c>
       <c r="G90">
-        <v>23443.39439124463</v>
+        <v>79011.85177188</v>
       </c>
       <c r="H90">
-        <v>36609.13463150214</v>
+        <v>44431.11394784</v>
       </c>
       <c r="I90">
-        <v>46.1729408491099</v>
+        <v>210.350100762596</v>
       </c>
       <c r="J90">
-        <v>143.7028654331695</v>
+        <v>166.9821093671459</v>
       </c>
     </row>
     <row r="91" spans="1:10">
       <c r="A91" s="1">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="B91">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="C91">
-        <v>79048.42849437706</v>
+        <v>43887.88875077467</v>
       </c>
       <c r="D91">
-        <v>44320.21433078919</v>
+        <v>44968.40922032659</v>
       </c>
       <c r="E91">
-        <v>329.7085657244825</v>
+        <v>-89.26070171115245</v>
       </c>
       <c r="F91">
-        <v>81</v>
+        <v>511</v>
       </c>
       <c r="G91">
-        <v>79011.85177188</v>
+        <v>43975.91750452055</v>
       </c>
       <c r="H91">
-        <v>44431.11394784</v>
+        <v>45056.16978643835</v>
       </c>
       <c r="I91">
-        <v>210.350100762596</v>
+        <v>-69.26377298904713</v>
       </c>
       <c r="J91">
-        <v>166.9821093671459</v>
+        <v>125.9001811302379</v>
       </c>
     </row>
     <row r="92" spans="1:10">
       <c r="A92" s="1">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="B92">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="C92">
-        <v>43887.88875077467</v>
+        <v>32028.20643276448</v>
       </c>
       <c r="D92">
-        <v>44968.40922032659</v>
+        <v>12600.75982004324</v>
       </c>
       <c r="E92">
-        <v>-89.26070171115245</v>
+        <v>37.82692056633449</v>
       </c>
       <c r="F92">
-        <v>511</v>
+        <v>51</v>
       </c>
       <c r="G92">
-        <v>43975.91750452055</v>
+        <v>31879.48173308</v>
       </c>
       <c r="H92">
-        <v>45056.16978643835</v>
+        <v>12739.63380402</v>
       </c>
       <c r="I92">
-        <v>-69.26377298904713</v>
+        <v>-5.124448294497238</v>
       </c>
       <c r="J92">
-        <v>125.9001811302379</v>
+        <v>207.965958293268</v>
       </c>
     </row>
     <row r="93" spans="1:10">
       <c r="A93" s="1">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="B93">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="C93">
-        <v>32028.20643276448</v>
+        <v>62498.57551508208</v>
       </c>
       <c r="D93">
-        <v>12600.75982004324</v>
+        <v>54556.17759076288</v>
       </c>
       <c r="E93">
-        <v>37.82692056633449</v>
+        <v>198.9816709359195</v>
       </c>
       <c r="F93">
-        <v>51</v>
+        <v>86</v>
       </c>
       <c r="G93">
-        <v>31879.48173308</v>
+        <v>62408.15493226</v>
       </c>
       <c r="H93">
-        <v>12739.63380402</v>
+        <v>54862.0108019</v>
       </c>
       <c r="I93">
-        <v>-5.124448294497238</v>
+        <v>49.59563391391228</v>
       </c>
       <c r="J93">
-        <v>207.965958293268</v>
+        <v>352.1732853148699</v>
       </c>
     </row>
     <row r="94" spans="1:10">
       <c r="A94" s="1">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="B94">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="C94">
-        <v>62498.57551508208</v>
+        <v>47983.95853431128</v>
       </c>
       <c r="D94">
-        <v>54556.17759076288</v>
+        <v>41336.18621893096</v>
       </c>
       <c r="E94">
-        <v>198.9816709359195</v>
+        <v>260.7593074863892</v>
       </c>
       <c r="F94">
-        <v>86</v>
+        <v>815</v>
       </c>
       <c r="G94">
-        <v>62408.15493226</v>
+        <v>46967.10636484849</v>
       </c>
       <c r="H94">
-        <v>54862.0108019</v>
+        <v>40996.69357439394</v>
       </c>
       <c r="I94">
-        <v>49.59563391391228</v>
+        <v>169.9855649525485</v>
       </c>
       <c r="J94">
-        <v>352.1732853148699</v>
+        <v>1075.86405394433</v>
       </c>
     </row>
     <row r="95" spans="1:10">
       <c r="A95" s="1">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="B95">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="C95">
-        <v>47983.95853431128</v>
+        <v>16821.79515573614</v>
       </c>
       <c r="D95">
-        <v>41336.18621893096</v>
+        <v>68381.14066238723</v>
       </c>
       <c r="E95">
-        <v>260.7593074863892</v>
+        <v>-82.82179395332324</v>
       </c>
       <c r="F95">
-        <v>815</v>
+        <v>30</v>
       </c>
       <c r="G95">
-        <v>46967.10636484849</v>
+        <v>16553.89760938</v>
       </c>
       <c r="H95">
-        <v>40996.69357439394</v>
+        <v>68640.79645304001</v>
       </c>
       <c r="I95">
-        <v>169.9855649525485</v>
+        <v>12.35421592270022</v>
       </c>
       <c r="J95">
-        <v>1075.86405394433</v>
+        <v>385.0307751584</v>
       </c>
     </row>
     <row r="96" spans="1:10">
       <c r="A96" s="1">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="B96">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="C96">
-        <v>16821.79515573614</v>
+        <v>25684.71096732826</v>
       </c>
       <c r="D96">
-        <v>68381.14066238723</v>
+        <v>41639.75120305002</v>
       </c>
       <c r="E96">
-        <v>-82.82179395332324</v>
+        <v>36.00829402977324</v>
       </c>
       <c r="F96">
-        <v>30</v>
+        <v>795</v>
       </c>
       <c r="G96">
-        <v>16553.89760938</v>
+        <v>25623.371062</v>
       </c>
       <c r="H96">
-        <v>68640.79645304001</v>
+        <v>41702.20162599999</v>
       </c>
       <c r="I96">
-        <v>12.35421592270022</v>
+        <v>21.758385044895</v>
       </c>
       <c r="J96">
-        <v>385.0307751584</v>
+        <v>88.68877729672212</v>
       </c>
     </row>
     <row r="97" spans="1:10">
       <c r="A97" s="1">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="B97">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="C97">
-        <v>25684.71096732826</v>
+        <v>74136.15095809012</v>
       </c>
       <c r="D97">
-        <v>41639.75120305002</v>
+        <v>67366.8999213068</v>
       </c>
       <c r="E97">
-        <v>36.00829402977324</v>
+        <v>119.6314421335978</v>
       </c>
       <c r="F97">
-        <v>795</v>
+        <v>13</v>
       </c>
       <c r="G97">
-        <v>25623.371062</v>
+        <v>73586.68309634567</v>
       </c>
       <c r="H97">
-        <v>41702.20162599999</v>
+        <v>67310.76477071605</v>
       </c>
       <c r="I97">
-        <v>21.758385044895</v>
+        <v>5.336586730254568</v>
       </c>
       <c r="J97">
-        <v>88.68877729672212</v>
+        <v>564.0296093234194</v>
       </c>
     </row>
     <row r="98" spans="1:10">
       <c r="A98" s="1">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="B98">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="C98">
-        <v>74136.15095809012</v>
+        <v>31248.43697171922</v>
       </c>
       <c r="D98">
-        <v>67366.8999213068</v>
+        <v>33615.58218444598</v>
       </c>
       <c r="E98">
-        <v>119.6314421335978</v>
+        <v>44.8719295477275</v>
       </c>
       <c r="F98">
-        <v>13</v>
+        <v>1669</v>
       </c>
       <c r="G98">
-        <v>73586.68309634567</v>
+        <v>31330.08882925</v>
       </c>
       <c r="H98">
-        <v>67310.76477071605</v>
+        <v>33715.487703</v>
       </c>
       <c r="I98">
-        <v>5.336586730254568</v>
+        <v>211.9397520159125</v>
       </c>
       <c r="J98">
-        <v>564.0296093234194</v>
+        <v>211.0919131090415</v>
       </c>
     </row>
     <row r="99" spans="1:10">
       <c r="A99" s="1">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="B99">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="C99">
-        <v>31248.43697171922</v>
+        <v>16673.29759542007</v>
       </c>
       <c r="D99">
-        <v>33615.58218444598</v>
+        <v>59916.7276261853</v>
       </c>
       <c r="E99">
-        <v>44.8719295477275</v>
+        <v>50.05779043594931</v>
       </c>
       <c r="F99">
-        <v>1669</v>
+        <v>277</v>
       </c>
       <c r="G99">
-        <v>31330.08882925</v>
+        <v>16599.3467168</v>
       </c>
       <c r="H99">
-        <v>33715.487703</v>
+        <v>59847.2891636</v>
       </c>
       <c r="I99">
-        <v>211.9397520159125</v>
+        <v>-137.127976950768</v>
       </c>
       <c r="J99">
-        <v>211.0919131090415</v>
+        <v>212.9059511780862</v>
       </c>
     </row>
     <row r="100" spans="1:10">
       <c r="A100" s="1">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="B100">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="C100">
-        <v>16673.29759542007</v>
+        <v>34188.80977234384</v>
       </c>
       <c r="D100">
-        <v>59916.7276261853</v>
+        <v>47602.82427002238</v>
       </c>
       <c r="E100">
-        <v>50.05779043594931</v>
+        <v>79.92086084630806</v>
       </c>
       <c r="F100">
-        <v>277</v>
+        <v>0</v>
       </c>
       <c r="G100">
-        <v>16599.3467168</v>
+        <v>34316.00229554324</v>
       </c>
       <c r="H100">
-        <v>59847.2891636</v>
+        <v>47940.29879731707</v>
       </c>
       <c r="I100">
-        <v>-137.127976950768</v>
+        <v>-123.1492064112602</v>
       </c>
       <c r="J100">
-        <v>212.9059511780862</v>
+        <v>413.8894136681935</v>
       </c>
     </row>
     <row r="101" spans="1:10">
       <c r="A101" s="1">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="B101">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="C101">
-        <v>34188.80977234384</v>
+        <v>38840.96072792721</v>
       </c>
       <c r="D101">
-        <v>47602.82427002238</v>
+        <v>50956.11790435812</v>
       </c>
       <c r="E101">
-        <v>79.92086084630806</v>
+        <v>-95.47899872551892</v>
       </c>
       <c r="F101">
-        <v>0</v>
+        <v>2103</v>
       </c>
       <c r="G101">
-        <v>34316.00229554324</v>
+        <v>38940.09785724138</v>
       </c>
       <c r="H101">
-        <v>47940.29879731707</v>
+        <v>50955.8674162069</v>
       </c>
       <c r="I101">
-        <v>-123.1492064112602</v>
+        <v>-35.20363653164552</v>
       </c>
       <c r="J101">
-        <v>413.8894136681935</v>
+        <v>116.0230685707424</v>
       </c>
     </row>
     <row r="102" spans="1:10">
       <c r="A102" s="1">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="B102">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="C102">
-        <v>38840.96072792721</v>
+        <v>35010.16893472205</v>
       </c>
       <c r="D102">
-        <v>50956.11790435812</v>
+        <v>68567.19053995087</v>
       </c>
       <c r="E102">
-        <v>-95.47899872551892</v>
+        <v>311.9364540204914</v>
       </c>
       <c r="F102">
-        <v>2103</v>
+        <v>880</v>
       </c>
       <c r="G102">
-        <v>38940.09785724138</v>
+        <v>34931.66292469194</v>
       </c>
       <c r="H102">
-        <v>50955.8674162069</v>
+        <v>68720.08543014218</v>
       </c>
       <c r="I102">
-        <v>-35.20363653164552</v>
+        <v>261.7047205180948</v>
       </c>
       <c r="J102">
-        <v>116.0230685707424</v>
+        <v>179.0621906157652</v>
       </c>
     </row>
     <row r="103" spans="1:10">
       <c r="A103" s="1">
-        <v>111</v>
+        <v>113</v>
       </c>
       <c r="B103">
-        <v>112</v>
+        <v>114</v>
       </c>
       <c r="C103">
-        <v>35010.16893472205</v>
+        <v>59096.11876235991</v>
       </c>
       <c r="D103">
-        <v>68567.19053995087</v>
+        <v>48018.84539025035</v>
       </c>
       <c r="E103">
-        <v>311.9364540204914</v>
+        <v>296.8030902833546</v>
       </c>
       <c r="F103">
-        <v>880</v>
+        <v>78</v>
       </c>
       <c r="G103">
-        <v>34931.66292469194</v>
+        <v>59145.52197381974</v>
       </c>
       <c r="H103">
-        <v>68720.08543014218</v>
+        <v>47883.11046017167</v>
       </c>
       <c r="I103">
-        <v>261.7047205180948</v>
+        <v>230.0223760579034</v>
       </c>
       <c r="J103">
-        <v>179.0621906157652</v>
+        <v>159.1361440354407</v>
       </c>
     </row>
     <row r="104" spans="1:10">
       <c r="A104" s="1">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="B104">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="C104">
-        <v>59096.11876235991</v>
+        <v>24787.41409324844</v>
       </c>
       <c r="D104">
-        <v>48018.84539025035</v>
+        <v>27154.4112100436</v>
       </c>
       <c r="E104">
-        <v>296.8030902833546</v>
+        <v>85.49353667554398</v>
       </c>
       <c r="F104">
-        <v>78</v>
+        <v>239</v>
       </c>
       <c r="G104">
-        <v>59145.52197381974</v>
+        <v>24643.18488685315</v>
       </c>
       <c r="H104">
-        <v>47883.11046017167</v>
+        <v>26580.08411149184</v>
       </c>
       <c r="I104">
-        <v>230.0223760579034</v>
+        <v>3.337898482102098</v>
       </c>
       <c r="J104">
-        <v>159.1361440354407</v>
+        <v>597.8321076985376</v>
       </c>
     </row>
     <row r="105" spans="1:10">
       <c r="A105" s="1">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="B105">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="C105">
-        <v>24787.41409324844</v>
+        <v>17995.4213301109</v>
       </c>
       <c r="D105">
-        <v>27154.4112100436</v>
+        <v>12191.86536336571</v>
       </c>
       <c r="E105">
-        <v>85.49353667554398</v>
+        <v>146.7861562788306</v>
       </c>
       <c r="F105">
-        <v>239</v>
+        <v>157</v>
       </c>
       <c r="G105">
-        <v>24643.18488685315</v>
+        <v>17769.21943090909</v>
       </c>
       <c r="H105">
-        <v>26580.08411149184</v>
+        <v>12303.53192590909</v>
       </c>
       <c r="I105">
-        <v>3.337898482102098</v>
+        <v>100.9991602774682</v>
       </c>
       <c r="J105">
-        <v>597.8321076985376</v>
+        <v>256.3848072635952</v>
       </c>
     </row>
     <row r="106" spans="1:10">
       <c r="A106" s="1">
-        <v>115</v>
+        <v>118</v>
       </c>
       <c r="B106">
-        <v>116</v>
+        <v>119</v>
       </c>
       <c r="C106">
-        <v>17995.4213301109</v>
+        <v>70119.7830401676</v>
       </c>
       <c r="D106">
-        <v>12191.86536336571</v>
+        <v>62338.66417011216</v>
       </c>
       <c r="E106">
-        <v>146.7861562788306</v>
+        <v>-4.615994815834384</v>
       </c>
       <c r="F106">
-        <v>157</v>
+        <v>2</v>
       </c>
       <c r="G106">
-        <v>17769.21943090909</v>
+        <v>70586.95735796</v>
       </c>
       <c r="H106">
-        <v>12303.53192590909</v>
+        <v>62046.04135962</v>
       </c>
       <c r="I106">
-        <v>100.9991602774682</v>
+        <v>61.51861753712922</v>
       </c>
       <c r="J106">
-        <v>256.3848072635952</v>
+        <v>555.2060332671027</v>
       </c>
     </row>
     <row r="107" spans="1:10">
       <c r="A107" s="1">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="B107">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="C107">
-        <v>70119.7830401676</v>
+        <v>17834.83015069988</v>
       </c>
       <c r="D107">
-        <v>62338.66417011216</v>
+        <v>63696.61609943701</v>
       </c>
       <c r="E107">
-        <v>-4.615994815834384</v>
+        <v>95.93194409014443</v>
       </c>
       <c r="F107">
-        <v>2</v>
+        <v>113</v>
       </c>
       <c r="G107">
-        <v>70586.95735796</v>
+        <v>17763.58562953238</v>
       </c>
       <c r="H107">
-        <v>62046.04135962</v>
+        <v>63714.94104776978</v>
       </c>
       <c r="I107">
-        <v>61.51861753712922</v>
+        <v>-118.0707674393795</v>
       </c>
       <c r="J107">
-        <v>555.2060332671027</v>
+        <v>226.2934954208227</v>
       </c>
     </row>
     <row r="108" spans="1:10">
       <c r="A108" s="1">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="B108">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="C108">
-        <v>17834.83015069988</v>
+        <v>68875.56043902965</v>
       </c>
       <c r="D108">
-        <v>63696.61609943701</v>
+        <v>38983.70369744477</v>
       </c>
       <c r="E108">
-        <v>95.93194409014443</v>
+        <v>153.7261490942617</v>
       </c>
       <c r="F108">
-        <v>113</v>
+        <v>680</v>
       </c>
       <c r="G108">
-        <v>17763.58562953238</v>
+        <v>69260.27935350724</v>
       </c>
       <c r="H108">
-        <v>63714.94104776978</v>
+        <v>39228.15446113043</v>
       </c>
       <c r="I108">
-        <v>-118.0707674393795</v>
+        <v>-78.48549220285059</v>
       </c>
       <c r="J108">
-        <v>226.2934954208227</v>
+        <v>511.5535801626451</v>
       </c>
     </row>
     <row r="109" spans="1:10">
       <c r="A109" s="1">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="B109">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="C109">
-        <v>68875.56043902965</v>
+        <v>6277.449716462531</v>
       </c>
       <c r="D109">
-        <v>38983.70369744477</v>
+        <v>41981.0008027181</v>
       </c>
       <c r="E109">
-        <v>153.7261490942617</v>
+        <v>-5.329617646144391</v>
       </c>
       <c r="F109">
-        <v>680</v>
+        <v>1678</v>
       </c>
       <c r="G109">
-        <v>69260.27935350724</v>
+        <v>6074.339510470589</v>
       </c>
       <c r="H109">
-        <v>39228.15446113043</v>
+        <v>42431.58889529412</v>
       </c>
       <c r="I109">
-        <v>-78.48549220285059</v>
+        <v>-49.17036520784823</v>
       </c>
       <c r="J109">
-        <v>511.5535801626451</v>
+        <v>496.1908867524158</v>
       </c>
     </row>
     <row r="110" spans="1:10">
       <c r="A110" s="1">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="B110">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="C110">
-        <v>6277.449716462531</v>
+        <v>38245.48393428839</v>
       </c>
       <c r="D110">
-        <v>41981.0008027181</v>
+        <v>70366.24719345206</v>
       </c>
       <c r="E110">
-        <v>-5.329617646144391</v>
+        <v>116.1198194443807</v>
       </c>
       <c r="F110">
-        <v>1678</v>
+        <v>23</v>
       </c>
       <c r="G110">
-        <v>6074.339510470589</v>
+        <v>38444.05776284</v>
       </c>
       <c r="H110">
-        <v>42431.58889529412</v>
+        <v>70508.30901482</v>
       </c>
       <c r="I110">
-        <v>-49.17036520784823</v>
+        <v>229.113267231244</v>
       </c>
       <c r="J110">
-        <v>496.1908867524158</v>
+        <v>269.0365137277552</v>
       </c>
     </row>
     <row r="111" spans="1:10">
       <c r="A111" s="1">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="B111">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="C111">
-        <v>38245.48393428839</v>
+        <v>33500.39950368611</v>
       </c>
       <c r="D111">
-        <v>70366.24719345206</v>
+        <v>52154.13537214541</v>
       </c>
       <c r="E111">
-        <v>116.1198194443807</v>
+        <v>135.3662865658088</v>
       </c>
       <c r="F111">
-        <v>23</v>
+        <v>187</v>
       </c>
       <c r="G111">
-        <v>38444.05776284</v>
+        <v>33384.68014169451</v>
       </c>
       <c r="H111">
-        <v>70508.30901482</v>
+        <v>52078.93322968973</v>
       </c>
       <c r="I111">
-        <v>229.113267231244</v>
+        <v>17.61254688233461</v>
       </c>
       <c r="J111">
-        <v>269.0365137277552</v>
+        <v>181.41740869914</v>
       </c>
     </row>
     <row r="112" spans="1:10">
       <c r="A112" s="1">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="B112">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="C112">
-        <v>33500.39950368611</v>
+        <v>63080.91901874998</v>
       </c>
       <c r="D112">
-        <v>52154.13537214541</v>
+        <v>30882.88800627405</v>
       </c>
       <c r="E112">
-        <v>135.3662865658088</v>
+        <v>185.6328097839708</v>
       </c>
       <c r="F112">
-        <v>187</v>
+        <v>7</v>
       </c>
       <c r="G112">
-        <v>33384.68014169451</v>
+        <v>63030.46892912467</v>
       </c>
       <c r="H112">
-        <v>52078.93322968973</v>
+        <v>30994.14253970822</v>
       </c>
       <c r="I112">
-        <v>17.61254688233461</v>
+        <v>68.62348358465815</v>
       </c>
       <c r="J112">
-        <v>181.41740869914</v>
+        <v>169.1566291059104</v>
       </c>
     </row>
     <row r="113" spans="1:10">
       <c r="A113" s="1">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="B113">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="C113">
-        <v>63080.91901874998</v>
+        <v>24583.7314694331</v>
       </c>
       <c r="D113">
-        <v>30882.88800627405</v>
+        <v>38466.42576023837</v>
       </c>
       <c r="E113">
-        <v>185.6328097839708</v>
+        <v>84.26767484467211</v>
       </c>
       <c r="F113">
-        <v>7</v>
+        <v>1774</v>
       </c>
       <c r="G113">
-        <v>63030.46892912467</v>
+        <v>24563.15365622642</v>
       </c>
       <c r="H113">
-        <v>30994.14253970822</v>
+        <v>38511.50608415094</v>
       </c>
       <c r="I113">
-        <v>68.62348358465815</v>
+        <v>156.5659636771585</v>
       </c>
       <c r="J113">
-        <v>169.1566291059104</v>
+        <v>87.65115269371786</v>
       </c>
     </row>
     <row r="114" spans="1:10">
       <c r="A114" s="1">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="B114">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="C114">
-        <v>24583.7314694331</v>
+        <v>60116.22108190351</v>
       </c>
       <c r="D114">
-        <v>38466.42576023837</v>
+        <v>46676.70761234349</v>
       </c>
       <c r="E114">
-        <v>84.26767484467211</v>
+        <v>128.2072964776129</v>
       </c>
       <c r="F114">
-        <v>1774</v>
+        <v>416</v>
       </c>
       <c r="G114">
-        <v>24563.15365622642</v>
+        <v>60038.28535125</v>
       </c>
       <c r="H114">
-        <v>38511.50608415094</v>
+        <v>46573.36035975</v>
       </c>
       <c r="I114">
-        <v>156.5659636771585</v>
+        <v>-0.03227196690975016</v>
       </c>
       <c r="J114">
-        <v>87.65115269371786</v>
+        <v>182.2087254934717</v>
       </c>
     </row>
     <row r="115" spans="1:10">
       <c r="A115" s="1">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="B115">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="C115">
-        <v>60116.22108190351</v>
+        <v>80138.45548056465</v>
       </c>
       <c r="D115">
-        <v>46676.70761234349</v>
+        <v>50137.37194649901</v>
       </c>
       <c r="E115">
-        <v>128.2072964776129</v>
+        <v>114.7910676899744</v>
       </c>
       <c r="F115">
-        <v>416</v>
+        <v>757</v>
       </c>
       <c r="G115">
-        <v>60038.28535125</v>
+        <v>80227.617138125</v>
       </c>
       <c r="H115">
-        <v>46573.36035975</v>
+        <v>50058.52061</v>
       </c>
       <c r="I115">
-        <v>-0.03227196690975016</v>
+        <v>-14.58793644055188</v>
       </c>
       <c r="J115">
-        <v>182.2087254934717</v>
+        <v>175.8017666475438</v>
       </c>
     </row>
     <row r="116" spans="1:10">
       <c r="A116" s="1">
-        <v>127</v>
+        <v>130</v>
       </c>
       <c r="B116">
-        <v>128</v>
+        <v>131</v>
       </c>
       <c r="C116">
-        <v>80138.45548056465</v>
+        <v>51634.30509151207</v>
       </c>
       <c r="D116">
-        <v>50137.37194649901</v>
+        <v>62577.66718996142</v>
       </c>
       <c r="E116">
-        <v>114.7910676899744</v>
+        <v>104.884742389008</v>
       </c>
       <c r="F116">
-        <v>757</v>
+        <v>14</v>
       </c>
       <c r="G116">
-        <v>80227.617138125</v>
+        <v>51945.43345061476</v>
       </c>
       <c r="H116">
-        <v>50058.52061</v>
+        <v>62660.97731069672</v>
       </c>
       <c r="I116">
-        <v>-14.58793644055188</v>
+        <v>-105.606160191042</v>
       </c>
       <c r="J116">
-        <v>175.8017666475438</v>
+        <v>384.7698690435958</v>
       </c>
     </row>
     <row r="117" spans="1:10">
       <c r="A117" s="1">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="B117">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="C117">
-        <v>51634.30509151207</v>
+        <v>22114.51252031825</v>
       </c>
       <c r="D117">
-        <v>62577.66718996142</v>
+        <v>63853.86207284085</v>
       </c>
       <c r="E117">
-        <v>104.884742389008</v>
+        <v>157.4461936754768</v>
       </c>
       <c r="F117">
-        <v>14</v>
+        <v>94</v>
       </c>
       <c r="G117">
-        <v>51945.43345061476</v>
+        <v>21442.5891727907</v>
       </c>
       <c r="H117">
-        <v>62660.97731069672</v>
+        <v>63930.88519383721</v>
       </c>
       <c r="I117">
-        <v>-105.606160191042</v>
+        <v>29.80754678913163</v>
       </c>
       <c r="J117">
-        <v>384.7698690435958</v>
+        <v>688.2624283655409</v>
       </c>
     </row>
     <row r="118" spans="1:10">
       <c r="A118" s="1">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="B118">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="C118">
-        <v>22114.51252031825</v>
+        <v>29494.89485955676</v>
       </c>
       <c r="D118">
-        <v>63853.86207284085</v>
+        <v>64133.47631382992</v>
       </c>
       <c r="E118">
-        <v>157.4461936754768</v>
+        <v>189.6060542432489</v>
       </c>
       <c r="F118">
-        <v>94</v>
+        <v>99</v>
       </c>
       <c r="G118">
-        <v>21442.5891727907</v>
+        <v>29445.26833648148</v>
       </c>
       <c r="H118">
-        <v>63930.88519383721</v>
+        <v>64079.35760709877</v>
       </c>
       <c r="I118">
-        <v>29.80754678913163</v>
+        <v>219.0325027710679</v>
       </c>
       <c r="J118">
-        <v>688.2624283655409</v>
+        <v>79.10462744842175</v>
       </c>
     </row>
     <row r="119" spans="1:10">
       <c r="A119" s="1">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="B119">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="C119">
-        <v>29494.89485955676</v>
+        <v>4663.523960649685</v>
       </c>
       <c r="D119">
-        <v>64133.47631382992</v>
+        <v>20219.63065549637</v>
       </c>
       <c r="E119">
-        <v>189.6060542432489</v>
+        <v>84.35517104410825</v>
       </c>
       <c r="F119">
-        <v>99</v>
+        <v>1417</v>
       </c>
       <c r="G119">
-        <v>29445.26833648148</v>
+        <v>6132.30469931579</v>
       </c>
       <c r="H119">
-        <v>64079.35760709877</v>
+        <v>19758.16929730263</v>
       </c>
       <c r="I119">
-        <v>219.0325027710679</v>
+        <v>165.6314339411026</v>
       </c>
       <c r="J119">
-        <v>79.10462744842175</v>
+        <v>1541.709854120762</v>
       </c>
     </row>
     <row r="120" spans="1:10">
       <c r="A120" s="1">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="B120">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="C120">
-        <v>4663.523960649685</v>
+        <v>16840.65715448542</v>
       </c>
       <c r="D120">
-        <v>20219.63065549637</v>
+        <v>36320.80747248431</v>
       </c>
       <c r="E120">
-        <v>84.35517104410825</v>
+        <v>-11.78328404060915</v>
       </c>
       <c r="F120">
-        <v>1417</v>
+        <v>1670</v>
       </c>
       <c r="G120">
-        <v>6132.30469931579</v>
+        <v>16552.71051225</v>
       </c>
       <c r="H120">
-        <v>19758.16929730263</v>
+        <v>36742.597276</v>
       </c>
       <c r="I120">
-        <v>165.6314339411026</v>
+        <v>4.409307706163003</v>
       </c>
       <c r="J120">
-        <v>1541.709854120762</v>
+        <v>510.9619429585096</v>
       </c>
     </row>
     <row r="121" spans="1:10">
       <c r="A121" s="1">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="B121">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="C121">
-        <v>16840.65715448542</v>
+        <v>5838.730894118888</v>
       </c>
       <c r="D121">
-        <v>36320.80747248431</v>
+        <v>43404.2363740681</v>
       </c>
       <c r="E121">
-        <v>-11.78328404060915</v>
+        <v>-2.96681082267943</v>
       </c>
       <c r="F121">
-        <v>1670</v>
+        <v>424</v>
       </c>
       <c r="G121">
-        <v>16552.71051225</v>
+        <v>5743.558804705883</v>
       </c>
       <c r="H121">
-        <v>36742.597276</v>
+        <v>43055.325</v>
       </c>
       <c r="I121">
-        <v>4.409307706163003</v>
+        <v>-46.76781496480589</v>
       </c>
       <c r="J121">
-        <v>510.9619429585096</v>
+        <v>364.3012510563055</v>
       </c>
     </row>
     <row r="122" spans="1:10">
       <c r="A122" s="1">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="B122">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="C122">
-        <v>5838.730894118888</v>
+        <v>11311.06100444165</v>
       </c>
       <c r="D122">
-        <v>43404.2363740681</v>
+        <v>44467.89160147071</v>
       </c>
       <c r="E122">
-        <v>-2.96681082267943</v>
+        <v>144.3014749350854</v>
       </c>
       <c r="F122">
-        <v>424</v>
+        <v>129</v>
       </c>
       <c r="G122">
-        <v>5743.558804705883</v>
+        <v>11401.92534981818</v>
       </c>
       <c r="H122">
-        <v>43055.325</v>
+        <v>44260.20501956363</v>
       </c>
       <c r="I122">
-        <v>-46.76781496480589</v>
+        <v>205.6582347177783</v>
       </c>
       <c r="J122">
-        <v>364.3012510563055</v>
+        <v>234.8503726545545</v>
       </c>
     </row>
     <row r="123" spans="1:10">
       <c r="A123" s="1">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="B123">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="C123">
-        <v>11311.06100444165</v>
+        <v>20902.28358425147</v>
       </c>
       <c r="D123">
-        <v>44467.89160147071</v>
+        <v>62722.22863611962</v>
       </c>
       <c r="E123">
-        <v>144.3014749350854</v>
+        <v>156.2117613166583</v>
       </c>
       <c r="F123">
-        <v>129</v>
+        <v>2029</v>
       </c>
       <c r="G123">
-        <v>11401.92534981818</v>
+        <v>21203.87051392857</v>
       </c>
       <c r="H123">
-        <v>44260.20501956363</v>
+        <v>62798.51253839286</v>
       </c>
       <c r="I123">
-        <v>205.6582347177783</v>
+        <v>26.47602884396589</v>
       </c>
       <c r="J123">
-        <v>234.8503726545545</v>
+        <v>337.0538090250853</v>
       </c>
     </row>
     <row r="124" spans="1:10">
       <c r="A124" s="1">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="B124">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="C124">
-        <v>20902.28358425147</v>
+        <v>64713.11257502079</v>
       </c>
       <c r="D124">
-        <v>62722.22863611962</v>
+        <v>33348.12302455684</v>
       </c>
       <c r="E124">
-        <v>156.2117613166583</v>
+        <v>181.0233578835553</v>
       </c>
       <c r="F124">
-        <v>2029</v>
+        <v>96</v>
       </c>
       <c r="G124">
-        <v>21203.87051392857</v>
+        <v>65239.58432513078</v>
       </c>
       <c r="H124">
-        <v>62798.51253839286</v>
+        <v>33650.86655758551</v>
       </c>
       <c r="I124">
-        <v>26.47602884396589</v>
+        <v>91.42890265615976</v>
       </c>
       <c r="J124">
-        <v>337.0538090250853</v>
+        <v>613.8837975236451</v>
       </c>
     </row>
     <row r="125" spans="1:10">
       <c r="A125" s="1">
-        <v>138</v>
+        <v>142</v>
       </c>
       <c r="B125">
-        <v>139</v>
+        <v>143</v>
       </c>
       <c r="C125">
-        <v>64713.11257502079</v>
+        <v>63561.11394846729</v>
       </c>
       <c r="D125">
-        <v>33348.12302455684</v>
+        <v>31882.11196468043</v>
       </c>
       <c r="E125">
-        <v>181.0233578835553</v>
+        <v>107.3154835694118</v>
       </c>
       <c r="F125">
-        <v>96</v>
+        <v>7</v>
       </c>
       <c r="G125">
-        <v>65239.58432513078</v>
+        <v>63030.46892912467</v>
       </c>
       <c r="H125">
-        <v>33650.86655758551</v>
+        <v>30994.14253970822</v>
       </c>
       <c r="I125">
-        <v>91.42890265615976</v>
+        <v>68.62348358465815</v>
       </c>
       <c r="J125">
-        <v>613.8837975236451</v>
+        <v>1035.167091392212</v>
       </c>
     </row>
     <row r="126" spans="1:10">
       <c r="A126" s="1">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="B126">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="C126">
-        <v>63561.11394846729</v>
+        <v>63871.73004353875</v>
       </c>
       <c r="D126">
-        <v>31882.11196468043</v>
+        <v>55804.21471317299</v>
       </c>
       <c r="E126">
-        <v>107.3154835694118</v>
+        <v>56.98562732968096</v>
       </c>
       <c r="F126">
-        <v>7</v>
+        <v>136</v>
       </c>
       <c r="G126">
-        <v>63030.46892912467</v>
+        <v>63714.75169168675</v>
       </c>
       <c r="H126">
-        <v>30994.14253970822</v>
+        <v>55358.1417454016</v>
       </c>
       <c r="I126">
-        <v>68.62348358465815</v>
+        <v>129.5216671956526</v>
       </c>
       <c r="J126">
-        <v>1035.167091392212</v>
+        <v>478.4190345356032</v>
       </c>
     </row>
     <row r="127" spans="1:10">
       <c r="A127" s="1">
-        <v>143</v>
+        <v>145</v>
       </c>
       <c r="B127">
-        <v>144</v>
+        <v>146</v>
       </c>
       <c r="C127">
-        <v>63871.73004353875</v>
+        <v>951.6854172142057</v>
       </c>
       <c r="D127">
-        <v>55804.21471317299</v>
+        <v>43284.46474882366</v>
       </c>
       <c r="E127">
-        <v>56.98562732968096</v>
+        <v>7.84271497128446</v>
       </c>
       <c r="F127">
-        <v>136</v>
+        <v>1022</v>
       </c>
       <c r="G127">
-        <v>63714.75169168675</v>
+        <v>313.7847049333333</v>
       </c>
       <c r="H127">
-        <v>55358.1417454016</v>
+        <v>43902.39077</v>
       </c>
       <c r="I127">
-        <v>129.5216671956526</v>
+        <v>-58.64537844487333</v>
       </c>
       <c r="J127">
-        <v>478.4190345356032</v>
+        <v>890.6012311586942</v>
       </c>
     </row>
     <row r="128" spans="1:10">
       <c r="A128" s="1">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="B128">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="C128">
-        <v>951.6854172142057</v>
+        <v>8682.663973852254</v>
       </c>
       <c r="D128">
-        <v>43284.46474882366</v>
+        <v>44623.14679867207</v>
       </c>
       <c r="E128">
-        <v>7.84271497128446</v>
+        <v>117.9814013222863</v>
       </c>
       <c r="F128">
-        <v>1022</v>
+        <v>246</v>
       </c>
       <c r="G128">
-        <v>313.7847049333333</v>
+        <v>8679.55087996206</v>
       </c>
       <c r="H128">
-        <v>43902.39077</v>
+        <v>44627.31232533875</v>
       </c>
       <c r="I128">
-        <v>-58.64537844487333</v>
+        <v>45.04295287680245</v>
       </c>
       <c r="J128">
-        <v>890.6012311586942</v>
+        <v>73.1235955599455</v>
       </c>
     </row>
     <row r="129" spans="1:10">
       <c r="A129" s="1">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="B129">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="C129">
-        <v>8682.663973852254</v>
+        <v>46417.65862238668</v>
       </c>
       <c r="D129">
-        <v>44623.14679867207</v>
+        <v>54480.9012222403</v>
       </c>
       <c r="E129">
-        <v>117.9814013222863</v>
+        <v>59.1026304713718</v>
       </c>
       <c r="F129">
-        <v>246</v>
+        <v>149</v>
       </c>
       <c r="G129">
-        <v>8679.55087996206</v>
+        <v>46234.22784679246</v>
       </c>
       <c r="H129">
-        <v>44627.31232533875</v>
+        <v>54722.1961803564</v>
       </c>
       <c r="I129">
-        <v>45.04295287680245</v>
+        <v>-64.97230666630063</v>
       </c>
       <c r="J129">
-        <v>73.1235955599455</v>
+        <v>327.5128948195298</v>
       </c>
     </row>
     <row r="130" spans="1:10">
       <c r="A130" s="1">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="B130">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="C130">
-        <v>46417.65862238668</v>
+        <v>50231.09881687512</v>
       </c>
       <c r="D130">
-        <v>54480.9012222403</v>
+        <v>54177.41894657805</v>
       </c>
       <c r="E130">
-        <v>59.1026304713718</v>
+        <v>-7.101061990793117</v>
       </c>
       <c r="F130">
-        <v>149</v>
+        <v>137</v>
       </c>
       <c r="G130">
-        <v>46234.22784679246</v>
+        <v>50508.97601096385</v>
       </c>
       <c r="H130">
-        <v>54722.1961803564</v>
+        <v>54342.86605728915</v>
       </c>
       <c r="I130">
-        <v>-64.97230666630063</v>
+        <v>-45.62328972018454</v>
       </c>
       <c r="J130">
-        <v>327.5128948195298</v>
+        <v>325.6876470892211</v>
       </c>
     </row>
     <row r="131" spans="1:10">
       <c r="A131" s="1">
-        <v>148</v>
+        <v>150</v>
       </c>
       <c r="B131">
-        <v>149</v>
+        <v>151</v>
       </c>
       <c r="C131">
-        <v>50231.09881687512</v>
+        <v>7753.371308554366</v>
       </c>
       <c r="D131">
-        <v>54177.41894657805</v>
+        <v>30164.46554301985</v>
       </c>
       <c r="E131">
-        <v>-7.101061990793117</v>
+        <v>103.6415643897835</v>
       </c>
       <c r="F131">
-        <v>137</v>
+        <v>77</v>
       </c>
       <c r="G131">
-        <v>50508.97601096385</v>
+        <v>7737.179169736111</v>
       </c>
       <c r="H131">
-        <v>54342.86605728915</v>
+        <v>31187.53680319445</v>
       </c>
       <c r="I131">
-        <v>-45.62328972018454</v>
+        <v>-4.164157812963611</v>
       </c>
       <c r="J131">
-        <v>325.6876470892211</v>
+        <v>1028.862995006821</v>
       </c>
     </row>
     <row r="132" spans="1:10">
       <c r="A132" s="1">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="B132">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="C132">
-        <v>7753.371308554366</v>
+        <v>71251.30221775151</v>
       </c>
       <c r="D132">
-        <v>30164.46554301985</v>
+        <v>42036.16701452169</v>
       </c>
       <c r="E132">
-        <v>103.6415643897835</v>
+        <v>-24.31715370972508</v>
       </c>
       <c r="F132">
-        <v>77</v>
+        <v>684</v>
       </c>
       <c r="G132">
-        <v>7737.179169736111</v>
+        <v>71317.05446650001</v>
       </c>
       <c r="H132">
-        <v>31187.53680319445</v>
+        <v>42174.755164</v>
       </c>
       <c r="I132">
-        <v>-4.164157812963611</v>
+        <v>-127.757975332035</v>
       </c>
       <c r="J132">
-        <v>1028.862995006821</v>
+        <v>185.0136129294411</v>
       </c>
     </row>
     <row r="133" spans="1:10">
       <c r="A133" s="1">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="B133">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="C133">
-        <v>71251.30221775151</v>
+        <v>71959.39443518301</v>
       </c>
       <c r="D133">
-        <v>42036.16701452169</v>
+        <v>78631.97153864655</v>
       </c>
       <c r="E133">
-        <v>-24.31715370972508</v>
+        <v>130.2184073459499</v>
       </c>
       <c r="F133">
-        <v>684</v>
+        <v>10</v>
       </c>
       <c r="G133">
-        <v>71317.05446650001</v>
+        <v>71882.93807845999</v>
       </c>
       <c r="H133">
-        <v>42174.755164</v>
+        <v>78181.44974954</v>
       </c>
       <c r="I133">
-        <v>-127.757975332035</v>
+        <v>-12.07565044334294</v>
       </c>
       <c r="J133">
-        <v>185.0136129294411</v>
+        <v>478.6053236491124</v>
       </c>
     </row>
     <row r="134" spans="1:10">
       <c r="A134" s="1">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="B134">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="C134">
-        <v>71959.39443518301</v>
+        <v>60672.22482565334</v>
       </c>
       <c r="D134">
-        <v>78631.97153864655</v>
+        <v>72167.72671662431</v>
       </c>
       <c r="E134">
-        <v>130.2184073459499</v>
+        <v>-21.21628525259476</v>
       </c>
       <c r="F134">
-        <v>10</v>
+        <v>197</v>
       </c>
       <c r="G134">
-        <v>71882.93807845999</v>
+        <v>60435.2151133657</v>
       </c>
       <c r="H134">
-        <v>78181.44974954</v>
+        <v>71955.97891893204</v>
       </c>
       <c r="I134">
-        <v>-12.07565044334294</v>
+        <v>-83.35540163580809</v>
       </c>
       <c r="J134">
-        <v>478.6053236491124</v>
+        <v>323.839471545834</v>
       </c>
     </row>
     <row r="135" spans="1:10">
       <c r="A135" s="1">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="B135">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="C135">
-        <v>60672.22482565334</v>
+        <v>67721.9595134445</v>
       </c>
       <c r="D135">
-        <v>72167.72671662431</v>
+        <v>37447.72129533788</v>
       </c>
       <c r="E135">
-        <v>-21.21628525259476</v>
+        <v>51.60420019211183</v>
       </c>
       <c r="F135">
-        <v>197</v>
+        <v>174</v>
       </c>
       <c r="G135">
-        <v>60435.2151133657</v>
+        <v>67558.11031111405</v>
       </c>
       <c r="H135">
-        <v>71955.97891893204</v>
+        <v>37355.09364092838</v>
       </c>
       <c r="I135">
-        <v>-83.35540163580809</v>
+        <v>137.7793207174533</v>
       </c>
       <c r="J135">
-        <v>323.839471545834</v>
+        <v>207.0086830625328</v>
       </c>
     </row>
     <row r="136" spans="1:10">
       <c r="A136" s="1">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="B136">
-        <v>155</v>
+        <v>157</v>
       </c>
       <c r="C136">
-        <v>67721.9595134445</v>
+        <v>4490.280545807043</v>
       </c>
       <c r="D136">
-        <v>37447.72129533788</v>
+        <v>29953.15735005216</v>
       </c>
       <c r="E136">
-        <v>51.60420019211183</v>
+        <v>-111.7113412436107</v>
       </c>
       <c r="F136">
-        <v>174</v>
+        <v>184</v>
       </c>
       <c r="G136">
-        <v>67558.11031111405</v>
+        <v>4464.247093328605</v>
       </c>
       <c r="H136">
-        <v>37355.09364092838</v>
+        <v>30106.98591111111</v>
       </c>
       <c r="I136">
-        <v>137.7793207174533</v>
+        <v>-54.98451660306958</v>
       </c>
       <c r="J136">
-        <v>207.0086830625328</v>
+        <v>166.0087331413995</v>
       </c>
     </row>
     <row r="137" spans="1:10">
       <c r="A137" s="1">
-        <v>155</v>
+        <v>157</v>
       </c>
       <c r="B137">
-        <v>157</v>
+        <v>159</v>
       </c>
       <c r="C137">
-        <v>4490.280545807043</v>
+        <v>73592.09115233978</v>
       </c>
       <c r="D137">
-        <v>29953.15735005216</v>
+        <v>36114.33939923555</v>
       </c>
       <c r="E137">
-        <v>-111.7113412436107</v>
+        <v>128.653312142246</v>
       </c>
       <c r="F137">
-        <v>184</v>
+        <v>101</v>
       </c>
       <c r="G137">
-        <v>4464.247093328605</v>
+        <v>74104.69195527054</v>
       </c>
       <c r="H137">
-        <v>30106.98591111111</v>
+        <v>36085.2197895992</v>
       </c>
       <c r="I137">
-        <v>-54.98451660306958</v>
+        <v>180.9019159912685</v>
       </c>
       <c r="J137">
-        <v>166.0087331413995</v>
+        <v>516.0789197737116</v>
       </c>
     </row>
     <row r="138" spans="1:10">
       <c r="A138" s="1">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="B138">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="C138">
-        <v>73592.09115233978</v>
+        <v>65949.36296047672</v>
       </c>
       <c r="D138">
-        <v>36114.33939923555</v>
+        <v>32274.63879730538</v>
       </c>
       <c r="E138">
-        <v>128.653312142246</v>
+        <v>136.0837178472835</v>
       </c>
       <c r="F138">
-        <v>101</v>
+        <v>79</v>
       </c>
       <c r="G138">
-        <v>74104.69195527054</v>
+        <v>65726.15615682327</v>
       </c>
       <c r="H138">
-        <v>36085.2197895992</v>
+        <v>31906.00885407159</v>
       </c>
       <c r="I138">
-        <v>180.9019159912685</v>
+        <v>276.6142441881723</v>
       </c>
       <c r="J138">
-        <v>516.0789197737116</v>
+        <v>453.2749067391516</v>
       </c>
     </row>
     <row r="139" spans="1:10">
       <c r="A139" s="1">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="B139">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="C139">
-        <v>65949.36296047672</v>
+        <v>46582.83852338985</v>
       </c>
       <c r="D139">
-        <v>32274.63879730538</v>
+        <v>57097.76153855612</v>
       </c>
       <c r="E139">
-        <v>136.0837178472835</v>
+        <v>195.145838400211</v>
       </c>
       <c r="F139">
-        <v>79</v>
+        <v>62</v>
       </c>
       <c r="G139">
-        <v>65726.15615682327</v>
+        <v>46462.12108883905</v>
       </c>
       <c r="H139">
-        <v>31906.00885407159</v>
+        <v>57003.98872036939</v>
       </c>
       <c r="I139">
-        <v>276.6142441881723</v>
+        <v>77.55059001400424</v>
       </c>
       <c r="J139">
-        <v>453.2749067391516</v>
+        <v>192.859230731179</v>
       </c>
     </row>
     <row r="140" spans="1:10">
       <c r="A140" s="1">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="B140">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="C140">
-        <v>46582.83852338985</v>
+        <v>37442.95592146718</v>
       </c>
       <c r="D140">
-        <v>57097.76153855612</v>
+        <v>34762.66311178004</v>
       </c>
       <c r="E140">
-        <v>195.145838400211</v>
+        <v>28.7707390874048</v>
       </c>
       <c r="F140">
-        <v>62</v>
+        <v>677</v>
       </c>
       <c r="G140">
-        <v>46462.12108883905</v>
+        <v>37272.86753739131</v>
       </c>
       <c r="H140">
-        <v>57003.98872036939</v>
+        <v>36110.06571956522</v>
       </c>
       <c r="I140">
-        <v>77.55059001400424</v>
+        <v>223.8359628803913</v>
       </c>
       <c r="J140">
-        <v>192.859230731179</v>
+        <v>1372.032903175881</v>
       </c>
     </row>
     <row r="141" spans="1:10">
       <c r="A141" s="1">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="B141">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="C141">
-        <v>37442.95592146718</v>
+        <v>14261.9960387133</v>
       </c>
       <c r="D141">
-        <v>34762.66311178004</v>
+        <v>27658.66076533399</v>
       </c>
       <c r="E141">
-        <v>28.7707390874048</v>
+        <v>126.2475390463561</v>
       </c>
       <c r="F141">
-        <v>677</v>
+        <v>115</v>
       </c>
       <c r="G141">
-        <v>37272.86753739131</v>
+        <v>14706.04005031579</v>
       </c>
       <c r="H141">
-        <v>36110.06571956522</v>
+        <v>27776.89932421053</v>
       </c>
       <c r="I141">
-        <v>223.8359628803913</v>
+        <v>-87.43471650237979</v>
       </c>
       <c r="J141">
-        <v>1372.032903175881</v>
+        <v>506.7697182958253</v>
       </c>
     </row>
     <row r="142" spans="1:10">
       <c r="A142" s="1">
-        <v>161</v>
+        <v>163</v>
       </c>
       <c r="B142">
-        <v>163</v>
+        <v>166</v>
       </c>
       <c r="C142">
-        <v>14261.9960387133</v>
+        <v>71349.76727104576</v>
       </c>
       <c r="D142">
-        <v>27658.66076533399</v>
+        <v>35027.8909495213</v>
       </c>
       <c r="E142">
-        <v>126.2475390463561</v>
+        <v>226.8170849306661</v>
       </c>
       <c r="F142">
-        <v>115</v>
+        <v>11</v>
       </c>
       <c r="G142">
-        <v>14706.04005031579</v>
+        <v>72409.87753564</v>
       </c>
       <c r="H142">
-        <v>27776.89932421053</v>
+        <v>35688.53038638</v>
       </c>
       <c r="I142">
-        <v>-87.43471650237979</v>
+        <v>120.7671043435914</v>
       </c>
       <c r="J142">
-        <v>506.7697182958253</v>
+        <v>1253.604737153453</v>
       </c>
     </row>
     <row r="143" spans="1:10">
       <c r="A143" s="1">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="B143">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="C143">
-        <v>71349.76727104576</v>
+        <v>19275.42204257387</v>
       </c>
       <c r="D143">
-        <v>35027.8909495213</v>
+        <v>53727.2195320763</v>
       </c>
       <c r="E143">
-        <v>226.8170849306661</v>
+        <v>148.6898653425666</v>
       </c>
       <c r="F143">
-        <v>11</v>
+        <v>1130</v>
       </c>
       <c r="G143">
-        <v>72409.87753564</v>
+        <v>19192.48909733333</v>
       </c>
       <c r="H143">
-        <v>35688.53038638</v>
+        <v>53987.98960666666</v>
       </c>
       <c r="I143">
-        <v>120.7671043435914</v>
+        <v>42.20918727788667</v>
       </c>
       <c r="J143">
-        <v>1253.604737153453</v>
+        <v>293.6273829349861</v>
       </c>
     </row>
     <row r="144" spans="1:10">
       <c r="A144" s="1">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="B144">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="C144">
-        <v>19275.42204257387</v>
+        <v>18726.52929306934</v>
       </c>
       <c r="D144">
-        <v>53727.2195320763</v>
+        <v>35983.22381475489</v>
       </c>
       <c r="E144">
-        <v>148.6898653425666</v>
+        <v>18.5600839396688</v>
       </c>
       <c r="F144">
-        <v>1130</v>
+        <v>175</v>
       </c>
       <c r="G144">
-        <v>19192.48909733333</v>
+        <v>18999.73747226107</v>
       </c>
       <c r="H144">
-        <v>53987.98960666666</v>
+        <v>36157.55644662004</v>
       </c>
       <c r="I144">
-        <v>42.20918727788667</v>
+        <v>-44.44769013936406</v>
       </c>
       <c r="J144">
-        <v>293.6273829349861</v>
+        <v>330.158379122339</v>
       </c>
     </row>
     <row r="145" spans="1:10">
       <c r="A145" s="1">
-        <v>165</v>
+        <v>167</v>
       </c>
       <c r="B145">
-        <v>168</v>
+        <v>170</v>
       </c>
       <c r="C145">
-        <v>18726.52929306934</v>
+        <v>79401.9187578597</v>
       </c>
       <c r="D145">
-        <v>35983.22381475489</v>
+        <v>39864.28347840362</v>
       </c>
       <c r="E145">
-        <v>18.5600839396688</v>
+        <v>226.0829533246574</v>
       </c>
       <c r="F145">
-        <v>175</v>
+        <v>2180</v>
       </c>
       <c r="G145">
-        <v>18999.73747226107</v>
+        <v>78363.916728</v>
       </c>
       <c r="H145">
-        <v>36157.55644662004</v>
+        <v>38736.572074</v>
       </c>
       <c r="I145">
-        <v>-44.44769013936406</v>
+        <v>353.1206123747</v>
       </c>
       <c r="J145">
-        <v>330.158379122339</v>
+        <v>1537.959619896361</v>
       </c>
     </row>
     <row r="146" spans="1:10">
       <c r="A146" s="1">
-        <v>167</v>
+        <v>169</v>
       </c>
       <c r="B146">
-        <v>170</v>
+        <v>172</v>
       </c>
       <c r="C146">
-        <v>79401.9187578597</v>
+        <v>49206.33590132581</v>
       </c>
       <c r="D146">
-        <v>39864.28347840362</v>
+        <v>42285.25087088904</v>
       </c>
       <c r="E146">
-        <v>226.0829533246574</v>
+        <v>246.5921931657016</v>
       </c>
       <c r="F146">
-        <v>2180</v>
+        <v>70</v>
       </c>
       <c r="G146">
-        <v>78363.916728</v>
+        <v>49086.11420782</v>
       </c>
       <c r="H146">
-        <v>38736.572074</v>
+        <v>42311.06911966</v>
       </c>
       <c r="I146">
-        <v>353.1206123747</v>
+        <v>177.672625494362</v>
       </c>
       <c r="J146">
-        <v>1537.959619896361</v>
+        <v>140.9600807569595</v>
       </c>
     </row>
     <row r="147" spans="1:10">
       <c r="A147" s="1">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="B147">
-        <v>172</v>
+        <v>174</v>
       </c>
       <c r="C147">
-        <v>49206.33590132581</v>
+        <v>2703.282633605787</v>
       </c>
       <c r="D147">
-        <v>42285.25087088904</v>
+        <v>18250.35172677296</v>
       </c>
       <c r="E147">
-        <v>246.5921931657016</v>
+        <v>49.31667749389352</v>
       </c>
       <c r="F147">
-        <v>70</v>
+        <v>204</v>
       </c>
       <c r="G147">
-        <v>49086.11420782</v>
+        <v>977.1797513162218</v>
       </c>
       <c r="H147">
-        <v>42311.06911966</v>
+        <v>18124.54063915811</v>
       </c>
       <c r="I147">
-        <v>177.672625494362</v>
+        <v>73.0757195840232</v>
       </c>
       <c r="J147">
-        <v>140.9600807569595</v>
+        <v>1730.844904113658</v>
       </c>
     </row>
     <row r="148" spans="1:10">
       <c r="A148" s="1">
-        <v>170</v>
+        <v>172</v>
       </c>
       <c r="B148">
-        <v>174</v>
+        <v>176</v>
       </c>
       <c r="C148">
-        <v>2703.282633605787</v>
+        <v>7659.197575523312</v>
       </c>
       <c r="D148">
-        <v>18250.35172677296</v>
+        <v>25050.96662333435</v>
       </c>
       <c r="E148">
-        <v>49.31667749389352</v>
+        <v>68.85792031657921</v>
       </c>
       <c r="F148">
-        <v>204</v>
+        <v>206</v>
       </c>
       <c r="G148">
-        <v>977.1797513162218</v>
+        <v>6440.852447036144</v>
       </c>
       <c r="H148">
-        <v>18124.54063915811</v>
+        <v>24334.83674759036</v>
       </c>
       <c r="I148">
-        <v>73.0757195840232</v>
+        <v>-6.253671089869393</v>
       </c>
       <c r="J148">
-        <v>1730.844904113658</v>
+        <v>1415.220336981176</v>
       </c>
     </row>
     <row r="149" spans="1:10">
       <c r="A149" s="1">
-        <v>172</v>
+        <v>174</v>
       </c>
       <c r="B149">
-        <v>176</v>
+        <v>178</v>
       </c>
       <c r="C149">
-        <v>7659.197575523312</v>
+        <v>16934.04791367867</v>
       </c>
       <c r="D149">
-        <v>25050.96662333435</v>
+        <v>75749.20730334366</v>
       </c>
       <c r="E149">
-        <v>68.85792031657921</v>
+        <v>69.14286618985457</v>
       </c>
       <c r="F149">
-        <v>206</v>
+        <v>126</v>
       </c>
       <c r="G149">
-        <v>6440.852447036144</v>
+        <v>17325.93627443609</v>
       </c>
       <c r="H149">
-        <v>24334.83674759036</v>
+        <v>75313.77939721805</v>
       </c>
       <c r="I149">
-        <v>-6.253671089869393</v>
+        <v>142.6206785263699</v>
       </c>
       <c r="J149">
-        <v>1415.220336981176</v>
+        <v>590.4006585665651</v>
       </c>
     </row>
     <row r="150" spans="1:10">
       <c r="A150" s="1">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="B150">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="C150">
-        <v>16934.04791367867</v>
+        <v>22151.34488759622</v>
       </c>
       <c r="D150">
-        <v>75749.20730334366</v>
+        <v>65281.49263279921</v>
       </c>
       <c r="E150">
-        <v>69.14286618985457</v>
+        <v>249.012218079772</v>
       </c>
       <c r="F150">
-        <v>126</v>
+        <v>34</v>
       </c>
       <c r="G150">
-        <v>17325.93627443609</v>
+        <v>22576.42121055794</v>
       </c>
       <c r="H150">
-        <v>75313.77939721805</v>
+        <v>66250.31412255365</v>
       </c>
       <c r="I150">
-        <v>142.6206785263699</v>
+        <v>148.3575623050889</v>
       </c>
       <c r="J150">
-        <v>590.4006585665651</v>
-      </c>
-    </row>
-    <row r="151" spans="1:10">
-      <c r="A151" s="1">
-        <v>175</v>
-      </c>
-      <c r="B151">
-        <v>179</v>
-      </c>
-      <c r="C151">
-        <v>22151.34488759622</v>
-      </c>
-      <c r="D151">
-        <v>65281.49263279921</v>
-      </c>
-      <c r="E151">
-        <v>249.012218079772</v>
-      </c>
-      <c r="F151">
-        <v>34</v>
-      </c>
-      <c r="G151">
-        <v>22576.42121055794</v>
-      </c>
-      <c r="H151">
-        <v>66250.31412255365</v>
-      </c>
-      <c r="I151">
-        <v>148.3575623050889</v>
-      </c>
-      <c r="J151">
         <v>1062.749414999504</v>
       </c>
     </row>

</xml_diff>